<commit_message>
Rebuild of output following PHN (composition-phn-1) fixes
 Rebuild of output following Personal Health Notes (composition-phn-1) fixes.
CIFMM-2807
</commit_message>
<xml_diff>
--- a/output/PersonalHealthRecords/composition-phn-1.xlsx
+++ b/output/PersonalHealthRecords/composition-phn-1.xlsx
@@ -3832,10 +3832,10 @@
       </c>
       <c r="P22" s="2"/>
       <c r="Q22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R22" t="s" s="2">
         <v>186</v>
-      </c>
-      <c r="R22" t="s" s="2">
-        <v>39</v>
       </c>
       <c r="S22" t="s" s="2">
         <v>39</v>
@@ -7714,10 +7714,10 @@
       </c>
       <c r="P58" s="2"/>
       <c r="Q58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R58" t="s" s="2">
         <v>371</v>
-      </c>
-      <c r="R58" t="s" s="2">
-        <v>39</v>
       </c>
       <c r="S58" t="s" s="2">
         <v>39</v>

</xml_diff>